<commit_message>
Se modifico el mapa de conceptos ahora son 4 aplicaciones diferentes, y se ampliaron los grafos a 4 tambien por cada app
</commit_message>
<xml_diff>
--- a/Trasporte.xlsx
+++ b/Trasporte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ingenieria de sistemas\Semestre 7\Ingenieria de software y requerimientos\Sistema_de_trasporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4342EE15-3D2D-47FC-A9FD-517374720083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2BF4B-3E28-48DB-A055-1192011004CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D12A9061-CC89-4189-9F90-E08A1FDB7012}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -174,9 +174,6 @@
     <t>el sistema le envia un mensaje de alerta al propietario de que el bus debe realizarse el debido mantenimiento, el propietario procede ha llevarlo a la revision tecnomicanica y que le hagan su respectivos arreglos, luego el propietario procede a subir el informe de mantenimiento a la plataforma para informar de que si se hizo.</t>
   </si>
   <si>
-    <t>el propietario esta dejando subir al bus a los usuarios, peor antes revisa en la lista de asientos vendidos  que las personas que estan ingresando si hayan pagado si no hacer el respectivo cobro, ademas de revisar que hayan hecho el chek in 0 contacto o si no proceder hacerlo antes de que suban al autobus</t>
-  </si>
-  <si>
     <t>hacer chek in a los usuarios</t>
   </si>
   <si>
@@ -220,6 +217,27 @@
   </si>
   <si>
     <t>El conductor entra al sistema de trasporte como conductor complementario, despues a listado de viajes y puede ver la hora, terminal donde debe recogerlo, datos del usuario, destino y si debe cobrarle en efectivo el viaje</t>
+  </si>
+  <si>
+    <t>Conductor</t>
+  </si>
+  <si>
+    <t>conductor</t>
+  </si>
+  <si>
+    <t>el Conductor esta dejando subir al bus a los usuarios, peor antes revisa en la lista de asientos vendidos  que las personas que estan ingresando si hayan pagado si no hacer el respectivo cobro, ademas de revisar que hayan hecho el chek in 0 contacto o si no proceder hacerlo antes de que suban al autobus</t>
+  </si>
+  <si>
+    <t>Centro de operaciones</t>
+  </si>
+  <si>
+    <t>atender PQR</t>
+  </si>
+  <si>
+    <t>poder dar respuesta a sus usuarios oconductores</t>
+  </si>
+  <si>
+    <t>el centro de operaciones reciben notificaciones de los usarios o conductores, este puede verlos y depues de esto puede darle una respuesta o generar una solucion con respecto a este PQR.</t>
   </si>
 </sst>
 </file>
@@ -337,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -362,9 +380,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -385,8 +400,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,25 +425,7 @@
   <dxfs count="10">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -449,7 +461,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -467,7 +479,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment wrapText="1"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -523,10 +535,28 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment wrapText="1"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -543,14 +573,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{752B708E-17DE-4C86-8BB0-632A45205642}" name="RF" displayName="RF" ref="A1:E15" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:E15" xr:uid="{C72AC1A9-14E4-48FD-B82A-B2096D0BF135}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{752B708E-17DE-4C86-8BB0-632A45205642}" name="RF" displayName="RF" ref="A1:E16" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E16" xr:uid="{C72AC1A9-14E4-48FD-B82A-B2096D0BF135}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{387612A3-9E8A-47B0-8C31-E264F4DDAC93}" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A47B53E6-97C2-4E81-8432-B63A0D6A4A93}" name="YO COMO" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{9900C71C-5722-4D95-ADEC-0E564318AC2D}" name="PUEDO" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A55F1E9B-E630-4063-8FF8-852212C366ED}" name="PARA" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6431491B-FA79-4667-A1D4-BBDE038D9267}" name="Historia de Usuario" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{387612A3-9E8A-47B0-8C31-E264F4DDAC93}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A47B53E6-97C2-4E81-8432-B63A0D6A4A93}" name="YO COMO" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9900C71C-5722-4D95-ADEC-0E564318AC2D}" name="PUEDO" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{A55F1E9B-E630-4063-8FF8-852212C366ED}" name="PARA" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{6431491B-FA79-4667-A1D4-BBDE038D9267}" name="Historia de Usuario" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,17 +883,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E0B388-141E-452E-82C6-AB5CC6ACFE9F}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="16.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="21" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="83.109375" style="3" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="3"/>
@@ -873,10 +903,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -890,10 +920,10 @@
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -907,10 +937,10 @@
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -924,13 +954,13 @@
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -941,10 +971,10 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -958,10 +988,10 @@
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -975,10 +1005,10 @@
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="19" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -992,27 +1022,27 @@
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1026,16 +1056,16 @@
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1043,16 +1073,16 @@
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1060,68 +1090,85 @@
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>48</v>
+      <c r="B12" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="D13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="C14" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>62</v>
+      <c r="B16" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifico Modelo_Requermientos.xlsx, se agregaron mas requerimientos
</commit_message>
<xml_diff>
--- a/Trasporte.xlsx
+++ b/Trasporte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ingenieria de sistemas\Semestre 7\Ingenieria de software y requerimientos\Sistema_de_trasporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2BF4B-3E28-48DB-A055-1192011004CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92FECBC-9D82-49ED-8F1B-F0DC0607344F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D12A9061-CC89-4189-9F90-E08A1FDB7012}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{D12A9061-CC89-4189-9F90-E08A1FDB7012}"/>
   </bookViews>
   <sheets>
     <sheet name="Historia de usuario" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -425,7 +428,7 @@
   <dxfs count="10">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -479,7 +482,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -577,10 +580,10 @@
   <autoFilter ref="A1:E16" xr:uid="{C72AC1A9-14E4-48FD-B82A-B2096D0BF135}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{387612A3-9E8A-47B0-8C31-E264F4DDAC93}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A47B53E6-97C2-4E81-8432-B63A0D6A4A93}" name="YO COMO" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9900C71C-5722-4D95-ADEC-0E564318AC2D}" name="PUEDO" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A47B53E6-97C2-4E81-8432-B63A0D6A4A93}" name="YO COMO" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{9900C71C-5722-4D95-ADEC-0E564318AC2D}" name="PUEDO" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{A55F1E9B-E630-4063-8FF8-852212C366ED}" name="PARA" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{6431491B-FA79-4667-A1D4-BBDE038D9267}" name="Historia de Usuario" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{6431491B-FA79-4667-A1D4-BBDE038D9267}" name="Historia de Usuario" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E0B388-141E-452E-82C6-AB5CC6ACFE9F}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>